<commit_message>
Changin fm load methods
</commit_message>
<xml_diff>
--- a/data/inputs/rcm.xlsx
+++ b/data/inputs/rcm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{75491DEA-6D8E-4AF6-B274-741D92C92968}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{64A763E4-30C6-42E5-B1D2-664807242E5E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,9 @@
     <sheet name="Inputs" sheetId="1" r:id="rId2"/>
     <sheet name="Failure Modes" sheetId="6" r:id="rId3"/>
     <sheet name="Tasks" sheetId="5" r:id="rId4"/>
-    <sheet name="brainstorming" sheetId="4" r:id="rId5"/>
-    <sheet name="units" sheetId="3" r:id="rId6"/>
+    <sheet name="Task Groups" sheetId="7" r:id="rId5"/>
+    <sheet name="brainstorming" sheetId="4" r:id="rId6"/>
+    <sheet name="units" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="105">
   <si>
     <t>component</t>
   </si>
@@ -258,6 +259,93 @@
   </si>
   <si>
     <t>repair</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>any</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>condition_loss</t>
+  </si>
+  <si>
+    <t>early_replacement</t>
+  </si>
+  <si>
+    <t>emergency_replacement</t>
+  </si>
+  <si>
+    <t>fungal decay</t>
+  </si>
+  <si>
+    <t>pole_saver_rod</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>[pole] {broken} due to (termites)</t>
+  </si>
+  <si>
+    <t>task_group</t>
+  </si>
+  <si>
+    <t>level_3_inspection</t>
+  </si>
+  <si>
+    <t>task_group_name</t>
+  </si>
+  <si>
+    <t>apportion_costs</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>maint</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Occas Thoughts</t>
+  </si>
+  <si>
+    <t>bearing example</t>
+  </si>
+  <si>
+    <t>Level of Failure</t>
+  </si>
+  <si>
+    <t>fm</t>
+  </si>
+  <si>
+    <t>component_1</t>
+  </si>
+  <si>
+    <t>asset_system</t>
+  </si>
+  <si>
+    <t>schedule</t>
+  </si>
+  <si>
+    <t>Completion</t>
+  </si>
+  <si>
+    <t>Schedule</t>
   </si>
 </sst>
 </file>
@@ -284,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,7 +411,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -356,14 +456,95 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -655,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,14 +1102,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4943E44-E3B0-4655-A8CA-2550CD88D719}">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:T1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="12.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -969,7 +1150,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -1091,7 +1272,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="E3" s="7">
         <v>50</v>
@@ -1103,9 +1284,15 @@
         <v>10</v>
       </c>
       <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="7">
+        <v>20</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
       <c r="L3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1185,66 +1372,106 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B045CC-E4FE-4549-979E-BE0104045CD6}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="9.140625" style="17"/>
+    <col min="19" max="19" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="9.140625" style="17"/>
+    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J1" s="16" t="s">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-    </row>
-    <row r="2" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="1" t="s">
+      <c r="W1" s="21"/>
+      <c r="X1" s="21"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+    </row>
+    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16" t="s">
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="1" t="s">
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-    </row>
-    <row r="3" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+    </row>
+    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1254,150 +1481,865 @@
       <c r="C3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="K3" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="Q3" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="R3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="S3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="T3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="U3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="V3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="W3" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="X3" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="Y3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="Z3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="AA3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="AB3" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="15">
         <v>0.8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="15">
+        <v>50</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="15">
         <v>20</v>
       </c>
-      <c r="I4">
+      <c r="J4" s="15">
         <v>5</v>
       </c>
-      <c r="J4" s="10" t="b">
+      <c r="K4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="P4" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="10" t="b">
+      <c r="Q4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="V4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="W4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB4" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F5" s="15">
+        <v>100</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>0</v>
-      </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8">
+      <c r="Q5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" s="19">
+        <v>50</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="V5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB5" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" s="19">
+        <v>50</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="V6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W6" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X6" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15">
+        <v>3500</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="P7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="19">
+        <v>0</v>
+      </c>
+      <c r="U7" s="19">
+        <v>50</v>
+      </c>
+      <c r="V7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X7" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" s="19">
+        <v>0</v>
+      </c>
+      <c r="U8" s="19">
+        <v>50</v>
+      </c>
+      <c r="V8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X8" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S9" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="20">
+        <v>0</v>
+      </c>
+      <c r="U9" s="20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="C10" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>7000</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R10" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="U10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="W10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X10" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+    </row>
+    <row r="12" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="16"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+    </row>
+    <row r="13" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="27"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="27"/>
+    </row>
+    <row r="14" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="15">
+        <v>50</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="15">
+        <v>20</v>
+      </c>
+      <c r="J14" s="15">
+        <v>5</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="P14" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="R14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="V14" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="W14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="X14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB14" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="15">
         <v>0.9</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F15" s="15">
+        <v>100</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" s="19">
+        <v>50</v>
+      </c>
+      <c r="U15" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="V15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA15" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB15" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="16"/>
+      <c r="S16" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T16" s="19">
+        <v>50</v>
+      </c>
+      <c r="U16" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="V16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X16" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <v>3500</v>
+      </c>
+      <c r="G17" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G8" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" t="b">
+      <c r="H17" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="P17" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="b">
+      <c r="Q17" s="16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="R17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T17" s="19">
+        <v>0</v>
+      </c>
+      <c r="U17" s="19">
+        <v>50</v>
+      </c>
+      <c r="V17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X17" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T18" s="19">
+        <v>0</v>
+      </c>
+      <c r="U18" s="19">
+        <v>50</v>
+      </c>
+      <c r="V18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="W18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="X18" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="T19" s="20">
+        <v>0</v>
+      </c>
+      <c r="U19" s="20">
+        <v>3</v>
+      </c>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+    </row>
+    <row r="20" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+      <c r="F20" s="15">
+        <v>7000</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D9">
+      <c r="P20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="R20" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>73</v>
+      <c r="S20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="T20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="U20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="V20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="W20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="X20" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+    </row>
+    <row r="21" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+      <c r="R21" s="16"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+    </row>
+    <row r="22" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P22" s="16"/>
+      <c r="Q22" s="16"/>
+      <c r="R22" s="16"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+    </row>
+    <row r="23" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="16"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+    </row>
+    <row r="24" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+      <c r="R24" s="16"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="19"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+    </row>
+    <row r="25" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+      <c r="R25" s="16"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+    </row>
+    <row r="26" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+      <c r="R26" s="16"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="19"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+    </row>
+    <row r="27" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+      <c r="R27" s="16"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="19"/>
+      <c r="V27" s="16"/>
+      <c r="W27" s="16"/>
+      <c r="X27" s="16"/>
+    </row>
+    <row r="28" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+      <c r="R28" s="16"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="19"/>
+      <c r="V28" s="16"/>
+      <c r="W28" s="16"/>
+      <c r="X28" s="16"/>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A8:B8 Y7:XFD8 S9 AC14:XFD20 F28:XFD28 E7:R7 E10:XFD13 E29:K30 M29:XFD30 L28:L30 E21:XFD27 E17:R17 E20:AB20 E15:AB16 E4:XFD6 A10:C17 A4:C7 A20:C30">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S7:X8">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A18:B18 Y17:AB18 S19 E14:F14 P14:AB14 H14:L14">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S17:X18">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14:O14">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1847B3D8-F642-4CC9-961A-746ED4B98939}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:J20"/>
   <sheetViews>
@@ -1477,7 +2419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
demo and task change
</commit_message>
<xml_diff>
--- a/data/inputs/rcm.xlsx
+++ b/data/inputs/rcm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5219A21D-4450-4A9E-95D3-35F744F14E38}"/>
+  <xr:revisionPtr revIDLastSave="1045" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{A4D155EB-4150-4452-892C-376F34765DE5}"/>
   <bookViews>
-    <workbookView xWindow="4395" yWindow="1545" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Failure Modes" sheetId="6" r:id="rId4"/>
     <sheet name="Indicators" sheetId="9" r:id="rId5"/>
     <sheet name="Tasks" sheetId="5" r:id="rId6"/>
-    <sheet name="DELETE" sheetId="12" r:id="rId7"/>
-    <sheet name="CostModel" sheetId="11" r:id="rId8"/>
+    <sheet name="CostModel" sheetId="11" r:id="rId7"/>
+    <sheet name="DELETE" sheetId="12" r:id="rId8"/>
     <sheet name="Task Groups" sheetId="7" r:id="rId9"/>
     <sheet name="brainstorming" sheetId="4" r:id="rId10"/>
     <sheet name="Sheet3" sheetId="10" r:id="rId11"/>
@@ -32,7 +32,7 @@
     <definedName name="ddIssue">[1]!TIssue[Issue]</definedName>
     <definedName name="ddReason">[1]!TReason[R1]</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="296">
   <si>
     <t>component</t>
   </si>
@@ -356,9 +356,6 @@
     <t>Schedule</t>
   </si>
   <si>
-    <t>Sate</t>
-  </si>
-  <si>
     <t>Impact</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
     <t>Footing</t>
   </si>
   <si>
-    <t>Simplified</t>
-  </si>
-  <si>
     <t>Pole Stay</t>
   </si>
   <si>
@@ -810,6 +804,138 @@
   </si>
   <si>
     <t>sf</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>FailureMode</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>as-bad-as-old</t>
+  </si>
+  <si>
+    <t>grp</t>
+  </si>
+  <si>
+    <t>reduction_factor</t>
+  </si>
+  <si>
+    <t>as_good_as_new</t>
+  </si>
+  <si>
+    <t>better_than_old_worse_than_new</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>Greg Discussion</t>
+  </si>
+  <si>
+    <t>Pole Footing</t>
+  </si>
+  <si>
+    <t>Task types -&gt; nomenclature</t>
+  </si>
+  <si>
+    <t>Failure Mode</t>
+  </si>
+  <si>
+    <t>rul_min</t>
+  </si>
+  <si>
+    <t>rul_max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>indicators</t>
+  </si>
+  <si>
+    <t>Asset Model</t>
+  </si>
+  <si>
+    <t>Asset Data</t>
+  </si>
+  <si>
+    <t>CAT1/2 replacement</t>
+  </si>
+  <si>
+    <t>CAT3/4 replacement</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>modify</t>
+  </si>
+  <si>
+    <t>addition</t>
+  </si>
+  <si>
+    <t>has_strut</t>
+  </si>
+  <si>
+    <t>value?</t>
+  </si>
+  <si>
+    <t>Greg -&gt; Life extension</t>
+  </si>
+  <si>
+    <t>Multiple tasks are triggered</t>
+  </si>
+  <si>
+    <t>reinforce</t>
+  </si>
+  <si>
+    <t>termite powder</t>
+  </si>
+  <si>
+    <t>life extension</t>
+  </si>
+  <si>
+    <t>change an indicator</t>
+  </si>
+  <si>
+    <t>Calibration scenario</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>kN</t>
+  </si>
+  <si>
+    <t>[pole top equipment] due to {cracking}</t>
+  </si>
+  <si>
+    <t>cracking_present</t>
+  </si>
+  <si>
+    <t>level_of_repair</t>
+  </si>
+  <si>
+    <t>as_bad_as_old</t>
   </si>
 </sst>
 </file>
@@ -819,7 +945,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -887,8 +1013,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -977,6 +1110,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -998,13 +1136,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1072,14 +1211,26 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{FE42BDC6-EBD5-43A7-A342-17D1DCC45724}"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1464,19 +1615,22 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A3:P42"/>
+  <dimension ref="A3:S71"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1484,7 +1638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1492,129 +1646,220 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="N6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>78</v>
+      </c>
+      <c r="S13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F14" s="12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>255</v>
+      </c>
+      <c r="S14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>25</v>
       </c>
       <c r="J15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>259</v>
+      </c>
+      <c r="S15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>258</v>
+      </c>
+      <c r="S16" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E31" t="s">
         <v>0</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O31" t="s">
-        <v>251</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="O31" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P31" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J32" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R32" t="s">
+        <v>78</v>
+      </c>
+      <c r="S32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>69</v>
       </c>
       <c r="K33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R33" t="s">
+        <v>255</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K34" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R34" t="s">
+        <v>259</v>
+      </c>
+      <c r="S34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35" t="s">
         <v>244</v>
       </c>
-      <c r="D35" t="s">
-        <v>246</v>
-      </c>
       <c r="G35" t="s">
+        <v>242</v>
+      </c>
+      <c r="L35" t="s">
         <v>244</v>
       </c>
-      <c r="L35" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="R35" t="s">
+        <v>258</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L36" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="R36" t="s">
+        <v>260</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D37" s="46" t="s">
         <v>52</v>
       </c>
@@ -1622,9 +1867,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E38" t="s">
         <v>65</v>
@@ -1633,32 +1878,170 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>243</v>
+      </c>
       <c r="E39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J39" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K42" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>4</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+      <c r="I54">
+        <v>10</v>
+      </c>
+      <c r="J54">
+        <f>PRODUCT(F54:I54)</f>
+        <v>480</v>
+      </c>
+      <c r="K54">
+        <v>60</v>
+      </c>
+      <c r="L54">
+        <f>K54*J54</f>
+        <v>28800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <f>L54/60/60</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>280</v>
+      </c>
+      <c r="E60" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>61</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>286</v>
+      </c>
+      <c r="B69">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>287</v>
+      </c>
+      <c r="B70">
+        <v>250</v>
+      </c>
+      <c r="C70" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>288</v>
+      </c>
+      <c r="B71">
+        <v>12.5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>289</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="O13:O15 O17:O18">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1680,48 +2063,48 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I5" s="3">
         <v>14</v>
@@ -1731,18 +2114,18 @@
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="R5" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="S5" t="s">
         <v>216</v>
-      </c>
-      <c r="S5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I6">
         <f>I5/4</f>
@@ -1754,51 +2137,51 @@
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I8" s="5">
         <v>320</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="S8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I9" s="5">
         <v>100</v>
@@ -1806,7 +2189,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -1814,12 +2197,12 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I12" s="9">
         <v>3.7</v>
@@ -1831,20 +2214,20 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="M16" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1048576" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048576" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2121,308 +2504,317 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B23F31-D664-4F99-AD97-38FA517354EE}">
-  <dimension ref="A2:M41"/>
+  <dimension ref="A2:T41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J2" s="1"/>
+      <c r="Q2" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="S2" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="T2" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="30" t="s">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q3" s="31"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>110</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="L3" t="s">
-        <v>234</v>
-      </c>
-      <c r="M3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="Q4" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="T6" s="34"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>262</v>
+      </c>
+      <c r="T7" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="J4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="J5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="34"/>
-      <c r="J6" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T10" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34" t="s">
+      <c r="T12" s="34"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="34"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34" t="s">
+      <c r="T14" s="34"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T15" t="s">
         <v>118</v>
       </c>
-      <c r="D14" s="34"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T16" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+    <row r="17" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="T17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="18" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q18" s="32"/>
+      <c r="R18" s="33" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33" t="s">
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+    </row>
+    <row r="19" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34" t="s">
+      <c r="T19" s="34"/>
+    </row>
+    <row r="20" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="T20" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="34"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q21" s="31"/>
+      <c r="S21" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="C21" t="s">
+    <row r="22" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q22" s="31"/>
+      <c r="T22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q23" s="31"/>
+      <c r="S23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="D22" t="s">
+    <row r="24" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q24" s="31"/>
+      <c r="T24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q25" s="31"/>
+      <c r="T25" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="C23" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="D24" t="s">
+    <row r="26" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q26" s="31"/>
+      <c r="S26" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="D25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="31"/>
-      <c r="C26" t="s">
+    <row r="27" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q27" s="31"/>
+      <c r="S27" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="C27" t="s">
+    <row r="28" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q28" s="31"/>
+      <c r="T28" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="31"/>
-      <c r="D28" t="s">
+    <row r="29" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q29" s="31"/>
+      <c r="S29" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="31"/>
-      <c r="C29" t="s">
+    <row r="30" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q30" s="31"/>
+      <c r="T30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q31" s="31"/>
+      <c r="T31" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
-      <c r="D30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="D31" t="s">
+    <row r="32" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q32" s="32"/>
+      <c r="R32" s="33" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="32"/>
-      <c r="B32" s="33" t="s">
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+    </row>
+    <row r="33" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34" t="s">
+      <c r="T33" s="34"/>
+    </row>
+    <row r="34" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q34" s="31"/>
+      <c r="T34" t="s">
         <v>134</v>
       </c>
-      <c r="D33" s="34"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="D34" t="s">
+    </row>
+    <row r="35" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q35" s="34"/>
+      <c r="R35" s="34"/>
+      <c r="S35" s="34" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34" t="s">
+      <c r="T35" s="34"/>
+    </row>
+    <row r="36" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q36" s="31"/>
+      <c r="T36" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="34"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="D36" t="s">
+    </row>
+    <row r="37" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q37" s="32"/>
+      <c r="R37" s="33" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="32"/>
-      <c r="B37" s="33" t="s">
+      <c r="S37" s="32"/>
+      <c r="T37" s="32"/>
+    </row>
+    <row r="38" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q38" s="34"/>
+      <c r="R38" s="34"/>
+      <c r="S38" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34" t="s">
+      <c r="T38" s="34"/>
+    </row>
+    <row r="39" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q39" s="31"/>
+      <c r="T39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="D38" s="34"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
-      <c r="D39" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="34"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34" t="s">
+      <c r="T40" s="34"/>
+    </row>
+    <row r="41" spans="17:20" x14ac:dyDescent="0.25">
+      <c r="Q41" s="31"/>
+      <c r="T41" t="s">
         <v>140</v>
-      </c>
-      <c r="D40" s="34"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
-      <c r="D41" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4943E44-E3B0-4655-A8CA-2550CD88D719}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,7 +2841,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2520,10 +2912,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2537,7 +2929,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -2549,7 +2941,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H6" t="s">
         <v>78</v>
@@ -2557,21 +2949,18 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -2594,13 +2983,10 @@
       <c r="H8" t="s">
         <v>21</v>
       </c>
-      <c r="J8" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E9" t="s">
         <v>84</v>
@@ -2608,13 +2994,10 @@
       <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E10" t="s">
         <v>84</v>
@@ -2625,18 +3008,15 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
-      <c r="J11" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B12">
         <v>1000</v>
@@ -2647,48 +3027,81 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="J12" t="s">
-        <v>45</v>
-      </c>
+      <c r="E12" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="45">
+        <v>20</v>
+      </c>
+      <c r="G12" s="45">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>230</v>
+      </c>
+      <c r="J12" s="48"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F13">
         <v>25</v>
       </c>
-      <c r="J13" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
-      </c>
-      <c r="J14" t="s">
-        <v>78</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
-      </c>
-      <c r="J15" t="s">
-        <v>78</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="17" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J17" t="s">
-        <v>78</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>231</v>
+      </c>
+      <c r="H19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>292</v>
+      </c>
+      <c r="B20">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>231</v>
+      </c>
+      <c r="H20" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -2701,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E4618E-A3DF-4EEC-9A86-F1390FA0DBB9}">
   <dimension ref="A2:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2714,10 +3127,10 @@
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>22</v>
@@ -2731,7 +3144,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2756,10 +3169,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -2768,26 +3181,26 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
         <v>78</v>
@@ -2795,7 +3208,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B8" t="s">
         <v>78</v>
@@ -2803,27 +3216,27 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -2833,7 +3246,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3">
@@ -2850,10 +3263,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B045CC-E4FE-4549-979E-BE0104045CD6}">
-  <dimension ref="A1:AB37"/>
+  <dimension ref="A1:AE33"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,20 +3276,21 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="9.140625" style="17"/>
-    <col min="19" max="19" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="9.140625" style="17"/>
-    <col min="25" max="25" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="9.140625" style="17"/>
+    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.140625" style="17"/>
+    <col min="28" max="28" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
@@ -2884,29 +3298,32 @@
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
       <c r="K1" s="25"/>
-      <c r="L1" s="2"/>
+      <c r="L1" s="25"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="22"/>
       <c r="R1" s="22"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="24"/>
-      <c r="U1" s="24"/>
-      <c r="V1" s="21" t="s">
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
+      <c r="Z1" s="21"/>
+      <c r="AA1" s="21"/>
       <c r="AB1" s="4"/>
-    </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+    </row>
+    <row r="2" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>76</v>
       </c>
@@ -2914,42 +3331,45 @@
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="25"/>
       <c r="K2" s="25"/>
-      <c r="L2" s="2" t="s">
+      <c r="L2" s="25"/>
+      <c r="M2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="23" t="s">
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="21" t="s">
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
+      <c r="AB2" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-    </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+    </row>
+    <row r="3" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2972,67 +3392,76 @@
         <v>54</v>
       </c>
       <c r="I3" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="J3" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="K3" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="L3" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="Q3" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="R3" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="S3" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="S3" s="23" t="s">
+      <c r="T3" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="U3" s="47" t="s">
+        <v>278</v>
+      </c>
+      <c r="V3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="24" t="s">
+      <c r="W3" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="24" t="s">
+      <c r="X3" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="Y3" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="Z3" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="X3" s="21" t="s">
+      <c r="AA3" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AB3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Z3" s="4" t="s">
+      <c r="AC3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AA3" s="4" t="s">
+      <c r="AD3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AB3" s="4" t="s">
+      <c r="AE3" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>9</v>
       </c>
@@ -3054,46 +3483,42 @@
       <c r="H4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="J4" s="15">
         <v>20</v>
       </c>
-      <c r="J4" s="15">
+      <c r="K4" s="15">
         <v>5</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="M4" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="N4" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="O4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="P4" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="P4" s="18" t="b">
+      <c r="Q4" s="18" t="b">
         <v>1</v>
-      </c>
-      <c r="Q4" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="R4" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="S4" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="T4" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="U4" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="V4" s="16" t="s">
+      <c r="S4" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="15" t="s">
         <v>78</v>
       </c>
       <c r="W4" s="18" t="s">
@@ -3102,7 +3527,7 @@
       <c r="X4" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="Y4" s="18" t="s">
+      <c r="Y4" s="16" t="s">
         <v>78</v>
       </c>
       <c r="Z4" s="18" t="s">
@@ -3114,8 +3539,17 @@
       <c r="AB4" s="18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE4" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="15" t="s">
         <v>72</v>
       </c>
@@ -3131,75 +3565,82 @@
       <c r="H5" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="I5" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="L5" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="P5" s="16" t="b">
-        <v>1</v>
       </c>
       <c r="Q5" s="16" t="b">
         <v>1</v>
       </c>
       <c r="R5" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="19">
+      <c r="W5" s="19">
         <v>50</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="X5" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="V5" s="16" t="b">
+      <c r="Y5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W5" s="16" t="b">
+      <c r="Z5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X5" s="16" t="b">
+      <c r="AA5" s="16" t="b">
         <v>0</v>
-      </c>
-      <c r="Y5" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z5" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA5" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="AB5" s="18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P6" s="16"/>
+      <c r="AC5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD5" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE5" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
-      <c r="S6" s="15" t="s">
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="T6" s="19">
+      <c r="W6" s="19">
         <v>50</v>
       </c>
-      <c r="U6" s="19" t="s">
+      <c r="X6" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="V6" s="16" t="b">
+      <c r="Y6" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W6" s="16" t="b">
+      <c r="Z6" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X6" s="16" t="b">
+      <c r="AA6" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E7" s="15">
         <v>1</v>
@@ -3213,99 +3654,110 @@
       <c r="H7" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="I7" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="L7" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="P7" s="16" t="b">
-        <v>1</v>
       </c>
       <c r="Q7" s="16" t="b">
         <v>1</v>
       </c>
       <c r="R7" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="S7" s="15" t="s">
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="T7" s="19">
+      <c r="W7" s="19">
         <v>0</v>
       </c>
-      <c r="U7" s="19">
+      <c r="X7" s="19">
         <v>50</v>
       </c>
-      <c r="V7" s="16" t="b">
+      <c r="Y7" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W7" s="16" t="b">
+      <c r="Z7" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X7" s="16" t="b">
+      <c r="AA7" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="S8" s="15" t="s">
+    <row r="8" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="19">
+      <c r="W8" s="19">
         <v>0</v>
       </c>
-      <c r="U8" s="19">
+      <c r="X8" s="19">
         <v>50</v>
       </c>
-      <c r="V8" s="16" t="b">
+      <c r="Y8" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W8" s="16" t="b">
+      <c r="Z8" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X8" s="16" t="b">
+      <c r="AA8" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="S9" s="15" t="s">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="V9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="20">
+      <c r="W9" s="20">
         <v>0</v>
       </c>
-      <c r="U9" s="20">
+      <c r="X9" s="20">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P10" s="16"/>
+    <row r="10" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
-      <c r="T10" s="19"/>
-      <c r="U10" s="19"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-    </row>
-    <row r="11" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P11" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="W10" s="19"/>
+      <c r="X10" s="19"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
+      <c r="AA10" s="16"/>
+    </row>
+    <row r="11" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
-      <c r="T11" s="19"/>
-      <c r="U11" s="19"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-    </row>
-    <row r="12" spans="1:28" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P12" s="27"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+    </row>
+    <row r="12" spans="1:31" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q12" s="27"/>
       <c r="R12" s="27"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-    </row>
-    <row r="13" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="U12" s="27"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+    </row>
+    <row r="13" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>9</v>
       </c>
@@ -3327,43 +3779,36 @@
       <c r="H13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="15">
+      <c r="J13" s="15">
         <v>20</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="15">
         <v>5</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="M13" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="N13" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="N13" s="15" t="s">
+      <c r="O13" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="P13" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="P13" s="18" t="b">
+      <c r="Q13" s="18" t="b">
         <v>1</v>
-      </c>
-      <c r="Q13" s="18" t="s">
-        <v>77</v>
       </c>
       <c r="R13" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="S13" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="T13" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="U13" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="V13" s="16" t="s">
+      <c r="S13" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="15" t="s">
         <v>78</v>
       </c>
       <c r="W13" s="18" t="s">
@@ -3372,7 +3817,7 @@
       <c r="X13" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="Y13" s="18" t="s">
+      <c r="Y13" s="16" t="s">
         <v>78</v>
       </c>
       <c r="Z13" s="18" t="s">
@@ -3384,8 +3829,17 @@
       <c r="AB13" s="18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="14" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD13" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE13" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
         <v>83</v>
       </c>
@@ -3401,70 +3855,74 @@
       <c r="H14" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="P14" s="16" t="b">
-        <v>1</v>
-      </c>
       <c r="Q14" s="16" t="b">
         <v>1</v>
       </c>
       <c r="R14" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="S14" s="15" t="s">
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="T14" s="19">
+      <c r="W14" s="19">
         <v>50</v>
       </c>
-      <c r="U14" s="19" t="s">
+      <c r="X14" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="V14" s="16" t="b">
+      <c r="Y14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W14" s="16" t="b">
+      <c r="Z14" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X14" s="16" t="b">
+      <c r="AA14" s="16" t="b">
         <v>0</v>
-      </c>
-      <c r="Y14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA14" s="18" t="s">
-        <v>78</v>
       </c>
       <c r="AB14" s="18" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P15" s="16"/>
+      <c r="AC14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE14" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
-      <c r="S15" s="15" t="s">
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="T15" s="19">
+      <c r="W15" s="19">
         <v>50</v>
       </c>
-      <c r="U15" s="19" t="s">
+      <c r="X15" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="V15" s="16" t="b">
+      <c r="Y15" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W15" s="16" t="b">
+      <c r="Z15" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X15" s="16" t="b">
+      <c r="AA15" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="15" t="s">
         <v>80</v>
       </c>
@@ -3480,55 +3938,57 @@
       <c r="H16" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="P16" s="16" t="b">
-        <v>1</v>
-      </c>
       <c r="Q16" s="16" t="b">
         <v>1</v>
       </c>
       <c r="R16" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="S16" s="15" t="s">
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="T16" s="19">
+      <c r="W16" s="19">
         <v>0</v>
       </c>
-      <c r="U16" s="19">
+      <c r="X16" s="19">
         <v>50</v>
       </c>
-      <c r="V16" s="16" t="b">
+      <c r="Y16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W16" s="16" t="b">
+      <c r="Z16" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X16" s="16" t="b">
+      <c r="AA16" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="S17" s="15" t="s">
+    <row r="17" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="T17" s="19">
+      <c r="W17" s="19">
         <v>0</v>
       </c>
-      <c r="U17" s="19">
+      <c r="X17" s="19">
         <v>50</v>
       </c>
-      <c r="V17" s="16" t="b">
+      <c r="Y17" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="W17" s="16" t="b">
+      <c r="Z17" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="X17" s="16" t="b">
+      <c r="AA17" s="16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -3543,27 +4003,30 @@
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
-      <c r="P18" s="17"/>
+      <c r="P18"/>
       <c r="Q18" s="17"/>
       <c r="R18" s="17"/>
-      <c r="S18" s="15" t="s">
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="T18" s="20">
+      <c r="W18" s="20">
         <v>0</v>
       </c>
-      <c r="U18" s="20">
+      <c r="X18" s="20">
         <v>3</v>
       </c>
-      <c r="V18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="17"/>
-      <c r="Y18"/>
-      <c r="Z18"/>
-      <c r="AA18"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
       <c r="AB18"/>
-    </row>
-    <row r="19" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+    </row>
+    <row r="19" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19" s="15" t="s">
@@ -3581,23 +4044,14 @@
       <c r="H19" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="P19" s="15" t="s">
-        <v>77</v>
-      </c>
       <c r="Q19" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="R19" s="15" t="b">
+      <c r="R19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="S19" s="15" t="b">
         <v>1</v>
-      </c>
-      <c r="S19" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="T19" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="U19" s="15" t="s">
-        <v>78</v>
       </c>
       <c r="V19" s="15" t="s">
         <v>78</v>
@@ -3608,158 +4062,249 @@
       <c r="X19" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="Y19"/>
-      <c r="Z19"/>
-      <c r="AA19"/>
+      <c r="Y19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z19" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA19" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="AB19"/>
-    </row>
-    <row r="20" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P20" s="16"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+    </row>
+    <row r="20" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="16"/>
-    </row>
-    <row r="21" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="16"/>
-    </row>
-    <row r="22" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P22" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="16"/>
+      <c r="AA20" s="16"/>
+    </row>
+    <row r="21" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="F21" s="15">
+        <v>50</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="L21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="P21" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="R21" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="U21" s="16"/>
+      <c r="V21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="W21" s="19">
+        <v>50</v>
+      </c>
+      <c r="X21" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC21" s="15">
+        <v>50</v>
+      </c>
+      <c r="AD21" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
-      <c r="T22" s="19"/>
-      <c r="U22" s="19"/>
-      <c r="V22" s="16"/>
-      <c r="W22" s="16"/>
-      <c r="X22" s="16"/>
-    </row>
-    <row r="23" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P23" s="16"/>
+      <c r="S22" s="16"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="W22" s="19">
+        <v>170</v>
+      </c>
+      <c r="X22" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA22" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB22" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC22" s="15">
+        <v>50</v>
+      </c>
+      <c r="AD22" s="16" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="16"/>
-      <c r="W23" s="16"/>
-      <c r="X23" s="16"/>
-    </row>
-    <row r="24" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P24" s="16"/>
+      <c r="S23" s="16"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="W23" s="19"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+    </row>
+    <row r="24" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
-      <c r="T24" s="19"/>
-      <c r="U24" s="19"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="16"/>
-    </row>
-    <row r="25" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P25" s="16"/>
+      <c r="S24" s="16"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="W24" s="19"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="16"/>
+    </row>
+    <row r="25" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
-      <c r="T25" s="19"/>
-      <c r="U25" s="19"/>
-      <c r="V25" s="16"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="16"/>
-    </row>
-    <row r="26" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="P26" s="16"/>
+      <c r="S25" s="16"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16"/>
+      <c r="AA25" s="16"/>
+    </row>
+    <row r="26" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
-      <c r="T26" s="19"/>
-      <c r="U26" s="19"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-    </row>
-    <row r="27" spans="1:28" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S26" s="16"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="W26" s="19"/>
+      <c r="X26" s="19"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16"/>
+      <c r="AA26" s="16"/>
+    </row>
+    <row r="27" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="P27" s="16"/>
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
-      <c r="T27" s="19"/>
-      <c r="U27" s="19"/>
-      <c r="V27" s="16"/>
-      <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="S27" s="16"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="16"/>
+      <c r="W27" s="19"/>
+      <c r="X27" s="19"/>
+      <c r="Y27" s="16"/>
+      <c r="Z27" s="16"/>
+      <c r="AA27" s="16"/>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>102</v>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A8:B8 Y7:XFD8 S9 AC13:XFD19 F27:XFD27 E7:R7 M28:XFD29 L27:L29 E20:XFD26 E16:R16 E19:AB19 E14:AB15 E4:XFD6 A4:C7 A19:C29 E28:E29 G28:K29 B35:B37 E10:XFD12 A10:C16">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="A8:B8 AB7:XFD8 V9 AF13:XFD19 F27:XFD27 E7:U7 N28:XFD29 M27:M29 E20:XFD26 E16:U16 E19:AE19 E14:AE15 E4:XFD6 A4:C7 A19:C29 E28:E29 G28:L29 E10:XFD12 A10:C16">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S7:X8">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="V7:AA8">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A17:B17 Y16:AB17 S18 E13:F13 P13:AB13 H13:L13">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+  <conditionalFormatting sqref="A17:B17 AB16:AE17 V18 E13:F13 Q13:AE13 H13:M13">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S16:X17">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="V16:AA17">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="M13">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M13:O13">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="N13:P13">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3769,6 +4314,230 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2045BA30-CA7E-4EE1-8F14-71E76892F009}">
+  <dimension ref="A2:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>100000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>52</v>
+      </c>
+      <c r="F7">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <f>D8*4</f>
+        <v>208</v>
+      </c>
+      <c r="F8">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>208</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>267</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>267</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>271</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>26</v>
+      </c>
+      <c r="F15">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D16">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16">
+        <v>7000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12C037A8-2E4B-4616-98B2-BA1E00D5199C}">
   <dimension ref="A2:D71"/>
   <sheetViews>
@@ -3805,242 +4574,242 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>144</v>
-      </c>
-      <c r="C4" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C6" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="37" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" s="37" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" s="37" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C13" s="37" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C14" s="37" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D15" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C19" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4063,77 +4832,77 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B22" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="C22" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D22" s="35" t="s">
         <v>161</v>
-      </c>
-      <c r="C22" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>161</v>
-      </c>
       <c r="C23" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="B24" s="35" t="s">
-        <v>161</v>
-      </c>
       <c r="C24" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B25" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D25" s="36" t="s">
         <v>164</v>
-      </c>
-      <c r="C25" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D25" s="36" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C26" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4147,92 +4916,92 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="C28" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D28" s="35" t="s">
         <v>168</v>
-      </c>
-      <c r="C28" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C29" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D29" s="36" t="s">
         <v>164</v>
-      </c>
-      <c r="C29" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C30" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C31" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C32" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="36" t="s">
-        <v>173</v>
-      </c>
       <c r="C33" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4246,77 +5015,77 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C35" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D35" s="36" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="C36" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D36" s="35" t="s">
         <v>175</v>
-      </c>
-      <c r="C36" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B37" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B37" s="36" t="s">
-        <v>175</v>
-      </c>
       <c r="C37" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C38" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B39" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="C39" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D39" s="36" t="s">
         <v>175</v>
-      </c>
-      <c r="C39" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D39" s="36" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4339,17 +5108,17 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B42" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D42" s="35" t="s">
         <v>164</v>
-      </c>
-      <c r="C42" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D42" s="35" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4363,242 +5132,242 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B44" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D45" s="36" t="s">
         <v>180</v>
-      </c>
-      <c r="B45" s="39" t="s">
-        <v>164</v>
-      </c>
-      <c r="C45" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D45" s="36" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C46" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D46" s="35" t="s">
         <v>182</v>
-      </c>
-      <c r="B46" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="C46" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="36" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C47" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C48" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C49" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D50" s="35" t="s">
         <v>185</v>
-      </c>
-      <c r="B50" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="C50" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D50" s="35" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B51" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C51" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C52" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C53" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D53" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C54" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C55" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D55" s="36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C56" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B57" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D57" s="36" t="s">
         <v>168</v>
-      </c>
-      <c r="C57" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D57" s="36" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B58" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C58" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B59" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="C59" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D59" s="36" t="s">
         <v>168</v>
-      </c>
-      <c r="C59" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D59" s="36" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4612,92 +5381,92 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D61" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B62" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C62" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B63" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" s="36" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D63" s="36" t="s">
         <v>161</v>
-      </c>
-      <c r="C63" s="36" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D63" s="36" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C64" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C65" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D65" s="36" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B66" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" s="35" t="e">
+        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
+        <v>#REF!</v>
+      </c>
+      <c r="D66" s="35" t="s">
         <v>164</v>
-      </c>
-      <c r="C66" s="35" t="e">
-        <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D66" s="35" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4720,47 +5489,47 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C69" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D69" s="36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B70" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C70" s="35" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D70" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C71" s="36" t="e">
         <f>IF(ISBLANK([1]!TRCM[[#This Row],[Issue]]),"",[1]!TRCM[[#Headers],[due to]])</f>
         <v>#REF!</v>
       </c>
       <c r="D71" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -4776,27 +5545,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2045BA30-CA7E-4EE1-8F14-71E76892F009}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1847B3D8-F642-4CC9-961A-746ED4B98939}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>